<commit_message>
[IMP] add 2 new reports
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -30,18 +30,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>รายงานการตรวจรับพัสดุประจำเดือน</t>
   </si>
   <si>
-    <t>ศุนย์</t>
-  </si>
-  <si>
     <t xml:space="preserve">วันที่ </t>
-  </si>
-  <si>
-    <t>ถึงวันที่</t>
   </si>
   <si>
     <t>เลขที่ใบเบิก</t>
@@ -86,11 +80,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,12 +103,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -140,27 +128,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC0C0C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC0C0C0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -193,91 +166,70 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -561,167 +513,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11" style="9" customWidth="1"/>
-    <col min="2" max="5" width="20" style="9" customWidth="1"/>
-    <col min="6" max="10" width="17.26953125" style="28" customWidth="1"/>
-    <col min="11" max="11" width="17.26953125" style="15" customWidth="1"/>
-    <col min="12" max="13" width="11.90625" style="15" customWidth="1"/>
-    <col min="14" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="11" style="6" customWidth="1"/>
+    <col min="2" max="5" width="20" style="6" customWidth="1"/>
+    <col min="6" max="10" width="17.33203125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="10" customWidth="1"/>
+    <col min="12" max="13" width="11.83203125" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="3"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="4"/>
     </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="5"/>
+      <c r="C5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="5"/>
+    <row r="6" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="L6">
+        <f>NETWORKDAYS(J6,K6)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" s="20" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="L7" s="15">
-        <f>NETWORKDAYS(J7,K7)</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="7" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:14" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="17" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="18" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="19" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="20" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="21" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="22" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="23" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="24" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="25" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="26" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="27" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="28" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="29" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="30" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="31" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
[IMP] Add new report and recondition
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Summary Report" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
[IMP] stock_request and sla balance report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_sla_balance.xlsx
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,6 +251,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -537,13 +546,14 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="4" customWidth="1"/>
-    <col min="2" max="5" width="20" style="4" customWidth="1"/>
+    <col min="2" max="4" width="20" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20" style="25" customWidth="1"/>
     <col min="6" max="10" width="17.33203125" style="15" customWidth="1"/>
     <col min="11" max="11" width="17.33203125" style="7" customWidth="1"/>
     <col min="12" max="13" width="11.83203125" style="7" customWidth="1"/>
@@ -557,7 +567,7 @@
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -575,7 +585,7 @@
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -593,7 +603,7 @@
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
@@ -611,7 +621,7 @@
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -627,7 +637,7 @@
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>

</xml_diff>